<commit_message>
Adding code to save posterior chains
</commit_message>
<xml_diff>
--- a/TablesResults.xlsx
+++ b/TablesResults.xlsx
@@ -215,12 +215,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1882,10 +1883,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:M96"/>
+  <dimension ref="B4:P96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B96" sqref="B4:M96"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="Q60" sqref="Q60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1963,32 +1964,32 @@
       <c r="C9" t="s">
         <v>1</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="G9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9">
+      <c r="D9" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3">
         <v>0.03</v>
       </c>
-      <c r="I9" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>0.161</v>
-      </c>
-      <c r="K9" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>0.95</v>
+      <c r="I9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0.94</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>22</v>
@@ -2001,32 +2002,32 @@
       <c r="C10" t="s">
         <v>1</v>
       </c>
-      <c r="D10">
-        <v>-1.01</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="G10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="I10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="K10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>0.96</v>
+      <c r="D10" s="3">
+        <v>-1.02</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0.91</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>22</v>
@@ -2039,32 +2040,32 @@
       <c r="C11" t="s">
         <v>1</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="G11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="I11" t="s">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>0.17299999999999999</v>
-      </c>
-      <c r="K11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>0.95</v>
+      <c r="D11" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0.96</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>22</v>
@@ -2074,11 +2075,29 @@
       <c r="B12" t="s">
         <v>20</v>
       </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>35</v>
       </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
       <c r="M13" s="2" t="s">
         <v>22</v>
       </c>
@@ -2087,28 +2106,51 @@
       <c r="B14" t="s">
         <v>20</v>
       </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>1</v>
       </c>
-      <c r="E15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K15" t="s">
-        <v>1</v>
-      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3"/>
       <c r="M15" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E16" t="s">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
@@ -2117,32 +2159,32 @@
       <c r="C17" t="s">
         <v>1</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>0.82599999999999996</v>
-      </c>
-      <c r="G17" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>1.024</v>
-      </c>
-      <c r="I17" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>1.024</v>
-      </c>
-      <c r="K17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>0.96</v>
+      <c r="D17" s="3">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.86394820000000005</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1.145</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1.006389</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0.94</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>22</v>
@@ -2155,32 +2197,32 @@
       <c r="C18" t="s">
         <v>1</v>
       </c>
-      <c r="D18">
-        <v>-1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>0.79900000000000004</v>
-      </c>
-      <c r="G18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="I18" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18">
-        <v>1.016</v>
-      </c>
-      <c r="K18" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <v>0.95</v>
+      <c r="D18" s="3">
+        <v>-1.01</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.72771410000000003</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.91731269999999998</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1.0017852</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0.94</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>22</v>
@@ -2193,32 +2235,32 @@
       <c r="C19" t="s">
         <v>1</v>
       </c>
-      <c r="D19">
-        <v>1.012</v>
-      </c>
-      <c r="E19" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>0.81699999999999995</v>
-      </c>
-      <c r="G19" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>1.0129999999999999</v>
-      </c>
-      <c r="I19" t="s">
-        <v>1</v>
-      </c>
-      <c r="J19">
-        <v>1.034</v>
-      </c>
-      <c r="K19" t="s">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>0.96</v>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.8851694</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3">
+        <v>1.1786916000000001</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1.0081467</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0.91</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>22</v>
@@ -2228,11 +2270,29 @@
       <c r="B20" t="s">
         <v>20</v>
       </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>36</v>
       </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
       <c r="M21" s="2" t="s">
         <v>22</v>
       </c>
@@ -2241,28 +2301,51 @@
       <c r="B22" t="s">
         <v>20</v>
       </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>1</v>
       </c>
-      <c r="E23" t="s">
-        <v>1</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K23" t="s">
-        <v>1</v>
-      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L23" s="3"/>
       <c r="M23" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E24" t="s">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
@@ -2271,31 +2354,31 @@
       <c r="C25" t="s">
         <v>1</v>
       </c>
-      <c r="D25">
-        <v>1.014</v>
-      </c>
-      <c r="E25" t="s">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>1.274</v>
-      </c>
-      <c r="G25" t="s">
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <v>1.2170000000000001</v>
-      </c>
-      <c r="I25" t="s">
-        <v>1</v>
-      </c>
-      <c r="J25">
-        <v>1.02</v>
-      </c>
-      <c r="K25" t="s">
-        <v>1</v>
-      </c>
-      <c r="L25">
+      <c r="D25" s="3">
+        <v>1.012</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1.2673798000000001</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3">
+        <v>1.342122</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25" s="3">
+        <v>1.0095664</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L25" s="3">
         <v>0.93</v>
       </c>
       <c r="M25" s="2" t="s">
@@ -2309,32 +2392,32 @@
       <c r="C26" t="s">
         <v>1</v>
       </c>
-      <c r="D26">
-        <v>-1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>1.099</v>
-      </c>
-      <c r="G26" t="s">
-        <v>1</v>
-      </c>
-      <c r="H26">
-        <v>1.0680000000000001</v>
-      </c>
-      <c r="I26" t="s">
-        <v>1</v>
-      </c>
-      <c r="J26">
-        <v>1.012</v>
-      </c>
-      <c r="K26" t="s">
-        <v>1</v>
-      </c>
-      <c r="L26">
-        <v>0.95</v>
+      <c r="D26" s="3">
+        <v>-1.016</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.87084379999999995</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0.85910299999999995</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0.9944655</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L26" s="3">
+        <v>0.93</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>22</v>
@@ -2347,32 +2430,32 @@
       <c r="C27" t="s">
         <v>1</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>1.08</v>
-      </c>
-      <c r="G27" t="s">
-        <v>1</v>
-      </c>
-      <c r="H27">
-        <v>1.071</v>
-      </c>
-      <c r="I27" t="s">
-        <v>1</v>
-      </c>
-      <c r="J27">
-        <v>1.014</v>
-      </c>
-      <c r="K27" t="s">
-        <v>1</v>
-      </c>
-      <c r="L27">
-        <v>0.95</v>
+      <c r="D27" s="3">
+        <v>1.016</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1.2145471000000001</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1.278627</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J27" s="3">
+        <v>1.001422</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L27" s="3">
+        <v>0.91</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>22</v>
@@ -2382,11 +2465,29 @@
       <c r="B28" t="s">
         <v>20</v>
       </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>37</v>
       </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
       <c r="M29" s="2" t="s">
         <v>22</v>
       </c>
@@ -2395,693 +2496,875 @@
       <c r="B30" t="s">
         <v>20</v>
       </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>1</v>
       </c>
-      <c r="E31" t="s">
-        <v>1</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="D31" s="3"/>
+      <c r="E31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K31" t="s">
-        <v>1</v>
-      </c>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L31" s="3"/>
       <c r="M31" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E32" t="s">
+      <c r="D32" s="3"/>
+      <c r="E32" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>21</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33" t="s">
-        <v>1</v>
-      </c>
-      <c r="F33">
-        <v>1.034</v>
-      </c>
-      <c r="G33" t="s">
-        <v>1</v>
-      </c>
-      <c r="H33">
-        <v>1.036</v>
-      </c>
-      <c r="I33" t="s">
-        <v>1</v>
-      </c>
-      <c r="J33">
-        <v>1.0189999999999999</v>
-      </c>
-      <c r="K33" t="s">
-        <v>1</v>
-      </c>
-      <c r="L33">
-        <v>0.96</v>
+      <c r="D33" s="3">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1.0017582</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33" s="3">
+        <v>1.0039966</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J33" s="3">
+        <v>1.0126751000000001</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L33" s="3">
+        <v>0.95</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>26</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
       </c>
-      <c r="D34">
-        <v>-1.0029999999999999</v>
-      </c>
-      <c r="E34" t="s">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>1.0209999999999999</v>
-      </c>
-      <c r="G34" t="s">
-        <v>1</v>
-      </c>
-      <c r="H34">
-        <v>1.0149999999999999</v>
-      </c>
-      <c r="I34" t="s">
-        <v>1</v>
-      </c>
-      <c r="J34">
-        <v>1.026</v>
-      </c>
-      <c r="K34" t="s">
-        <v>1</v>
-      </c>
-      <c r="L34">
-        <v>0.95</v>
+      <c r="D34" s="3">
+        <v>-1.012</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.96707670000000001</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0.97095730000000002</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J34" s="3">
+        <v>1.0079088</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L34" s="3">
+        <v>0.92</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>27</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
       </c>
-      <c r="D35">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="E35" t="s">
-        <v>1</v>
-      </c>
-      <c r="F35">
-        <v>1.022</v>
-      </c>
-      <c r="G35" t="s">
-        <v>1</v>
-      </c>
-      <c r="H35">
-        <v>1.044</v>
-      </c>
-      <c r="I35" t="s">
-        <v>1</v>
-      </c>
-      <c r="J35">
-        <v>1.034</v>
-      </c>
-      <c r="K35" t="s">
-        <v>1</v>
-      </c>
-      <c r="L35">
+      <c r="D35" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="3">
+        <v>1.0065158999999999</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H35" s="3">
+        <v>1.0205786999999999</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J35" s="3">
+        <v>1.0035689000000001</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L35" s="3">
         <v>0.95</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>45</v>
       </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
       <c r="M37" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>28</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
       </c>
-      <c r="D39">
-        <v>1.145</v>
-      </c>
-      <c r="E39" t="s">
-        <v>1</v>
-      </c>
-      <c r="F39">
-        <v>0.156</v>
-      </c>
-      <c r="G39" t="s">
-        <v>1</v>
-      </c>
-      <c r="H39">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="I39" t="s">
-        <v>1</v>
-      </c>
-      <c r="J39">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="K39" t="s">
-        <v>1</v>
-      </c>
-      <c r="L39">
-        <v>0.23</v>
+      <c r="D39" s="3">
+        <v>1.212</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.218</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J39" s="3">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L39" s="3">
+        <v>0.02</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>29</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
       </c>
-      <c r="D40">
-        <v>-0.52500000000000002</v>
-      </c>
-      <c r="E40" t="s">
-        <v>1</v>
-      </c>
-      <c r="F40">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="G40" t="s">
-        <v>1</v>
-      </c>
-      <c r="H40">
+      <c r="D40" s="3">
+        <v>-0.52400000000000002</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F40" s="3">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H40" s="3">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="I40" t="s">
-        <v>1</v>
-      </c>
-      <c r="J40">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="K40" t="s">
-        <v>1</v>
-      </c>
-      <c r="L40">
-        <v>0.95</v>
+      <c r="I40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J40" s="3">
+        <v>0.154</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L40" s="3">
+        <v>0.9</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>30</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
       </c>
-      <c r="D41">
-        <v>0.439</v>
-      </c>
-      <c r="E41" t="s">
-        <v>1</v>
-      </c>
-      <c r="F41">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="G41" t="s">
-        <v>1</v>
-      </c>
-      <c r="H41">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="I41" t="s">
-        <v>1</v>
-      </c>
-      <c r="J41">
-        <v>0.18</v>
-      </c>
-      <c r="K41" t="s">
-        <v>1</v>
-      </c>
-      <c r="L41">
-        <v>0.73</v>
+      <c r="D41" s="3">
+        <v>-1.4610000000000001</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J41" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L41" s="3">
+        <v>0.28999999999999998</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>38</v>
       </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
       <c r="M43" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
         <v>1</v>
       </c>
-      <c r="E45" t="s">
-        <v>1</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="D45" s="3"/>
+      <c r="E45" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K45" t="s">
-        <v>1</v>
-      </c>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L45" s="3"/>
       <c r="M45" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E46" t="s">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D46" s="3"/>
+      <c r="E46" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>28</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
       </c>
-      <c r="D47">
-        <v>0.83699999999999997</v>
-      </c>
-      <c r="E47" t="s">
-        <v>1</v>
-      </c>
-      <c r="F47">
-        <v>1.069</v>
-      </c>
-      <c r="G47" t="s">
-        <v>1</v>
-      </c>
-      <c r="H47">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="I47" t="s">
-        <v>1</v>
-      </c>
-      <c r="J47">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="K47" t="s">
-        <v>1</v>
-      </c>
-      <c r="L47">
+      <c r="D47" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3">
+        <v>1.6056345000000001</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H47" s="3">
+        <v>1.6485304000000001</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J47" s="3">
+        <v>0.57272469999999998</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L47" s="3">
         <v>0</v>
       </c>
       <c r="M47" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P47" s="1"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>29</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
       </c>
-      <c r="D48">
-        <v>-0.186</v>
-      </c>
-      <c r="E48" t="s">
-        <v>1</v>
-      </c>
-      <c r="F48">
-        <v>7.0990000000000002</v>
-      </c>
-      <c r="G48" t="s">
-        <v>1</v>
-      </c>
-      <c r="H48">
-        <v>8.3770000000000007</v>
-      </c>
-      <c r="I48" t="s">
-        <v>1</v>
-      </c>
-      <c r="J48">
-        <v>0.67800000000000005</v>
-      </c>
-      <c r="K48" t="s">
-        <v>1</v>
-      </c>
-      <c r="L48">
+      <c r="D48" s="3">
+        <v>-0.20300000000000001</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3">
+        <v>6.3081459000000004</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H48" s="3">
+        <v>7.9252786000000004</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J48" s="3">
+        <v>0.71707580000000004</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L48" s="3">
         <v>0</v>
       </c>
       <c r="M48" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P48" s="1"/>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>30</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>
       </c>
-      <c r="D49">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="E49" t="s">
-        <v>1</v>
-      </c>
-      <c r="F49">
-        <v>3.7639999999999998</v>
-      </c>
-      <c r="G49" t="s">
-        <v>1</v>
-      </c>
-      <c r="H49">
-        <v>4.4320000000000004</v>
-      </c>
-      <c r="I49" t="s">
-        <v>1</v>
-      </c>
-      <c r="J49">
-        <v>0.76300000000000001</v>
-      </c>
-      <c r="K49" t="s">
-        <v>1</v>
-      </c>
-      <c r="L49">
+      <c r="D49" s="3">
+        <v>-0.46500000000000002</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3">
+        <v>4.2236545000000003</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H49" s="3">
+        <v>4.5595471999999999</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J49" s="3">
+        <v>0.52540480000000001</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L49" s="3">
         <v>0</v>
       </c>
       <c r="M49" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P49" s="1"/>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="P50" s="1"/>
+    </row>
+    <row r="51" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>39</v>
       </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
       <c r="M51" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P51" s="1"/>
+    </row>
+    <row r="52" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="P52" s="1"/>
+    </row>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
         <v>1</v>
       </c>
-      <c r="E53" t="s">
-        <v>1</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="D53" s="3"/>
+      <c r="E53" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K53" t="s">
-        <v>1</v>
-      </c>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L53" s="3"/>
       <c r="M53" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E54" t="s">
+      <c r="P53" s="1"/>
+    </row>
+    <row r="54" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D54" s="3"/>
+      <c r="E54" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="P54" s="1"/>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>28</v>
       </c>
       <c r="C55" t="s">
         <v>1</v>
       </c>
-      <c r="D55">
-        <v>1.2390000000000001</v>
-      </c>
-      <c r="E55" t="s">
-        <v>1</v>
-      </c>
-      <c r="F55">
-        <v>1.59</v>
-      </c>
-      <c r="G55" t="s">
-        <v>1</v>
-      </c>
-      <c r="H55">
-        <v>1.639</v>
-      </c>
-      <c r="I55" t="s">
-        <v>1</v>
-      </c>
-      <c r="J55">
-        <v>1.369</v>
-      </c>
-      <c r="K55" t="s">
-        <v>1</v>
-      </c>
-      <c r="L55">
-        <v>0.04</v>
+      <c r="D55" s="3">
+        <v>1.302</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F55" s="3">
+        <v>1.4197869999999999</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H55" s="3">
+        <v>1.4248970000000001</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J55" s="3">
+        <v>1.1361718000000001</v>
+      </c>
+      <c r="K55" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L55" s="3">
+        <v>0</v>
       </c>
       <c r="M55" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P55" s="1"/>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>29</v>
       </c>
       <c r="C56" t="s">
         <v>1</v>
       </c>
-      <c r="D56">
-        <v>-0.34100000000000003</v>
-      </c>
-      <c r="E56" t="s">
-        <v>1</v>
-      </c>
-      <c r="F56">
-        <v>3.7970000000000002</v>
-      </c>
-      <c r="G56" t="s">
-        <v>1</v>
-      </c>
-      <c r="H56">
-        <v>4.2329999999999997</v>
-      </c>
-      <c r="I56" t="s">
-        <v>1</v>
-      </c>
-      <c r="J56">
-        <v>1.4790000000000001</v>
-      </c>
-      <c r="K56" t="s">
-        <v>1</v>
-      </c>
-      <c r="L56">
-        <v>0.25</v>
+      <c r="D56" s="3">
+        <v>-0.38700000000000001</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F56" s="3">
+        <v>2.5810968000000001</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H56" s="3">
+        <v>3.008283</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J56" s="3">
+        <v>1.1759295999999999</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L56" s="3">
+        <v>0.36</v>
       </c>
       <c r="M56" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>30</v>
       </c>
       <c r="C57" t="s">
         <v>1</v>
       </c>
-      <c r="D57">
-        <v>0.34899999999999998</v>
-      </c>
-      <c r="E57" t="s">
-        <v>1</v>
-      </c>
-      <c r="F57">
-        <v>2.0219999999999998</v>
-      </c>
-      <c r="G57" t="s">
-        <v>1</v>
-      </c>
-      <c r="H57">
-        <v>2.25</v>
-      </c>
-      <c r="I57" t="s">
-        <v>1</v>
-      </c>
-      <c r="J57">
-        <v>1.3380000000000001</v>
-      </c>
-      <c r="K57" t="s">
-        <v>1</v>
-      </c>
-      <c r="L57">
-        <v>0.28999999999999998</v>
+      <c r="D57" s="3">
+        <v>-1.4239999999999999</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F57" s="3">
+        <v>1.3401611</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H57" s="3">
+        <v>1.3859570000000001</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J57" s="3">
+        <v>1.0923901</v>
+      </c>
+      <c r="K57" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L57" s="3">
+        <v>0.09</v>
       </c>
       <c r="M57" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+    </row>
+    <row r="59" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>40</v>
       </c>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
       <c r="M59" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+    </row>
+    <row r="61" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
         <v>1</v>
       </c>
-      <c r="E61" t="s">
-        <v>1</v>
-      </c>
-      <c r="F61" t="s">
+      <c r="D61" s="3"/>
+      <c r="E61" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K61" t="s">
-        <v>1</v>
-      </c>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L61" s="3"/>
       <c r="M61" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E62" t="s">
+    <row r="62" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D62" s="3"/>
+      <c r="E62" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+    </row>
+    <row r="63" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>28</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
       </c>
-      <c r="D63">
-        <v>1.3149999999999999</v>
-      </c>
-      <c r="E63" t="s">
-        <v>1</v>
-      </c>
-      <c r="F63">
-        <v>2.052</v>
-      </c>
-      <c r="G63" t="s">
-        <v>1</v>
-      </c>
-      <c r="H63">
-        <v>2.16</v>
-      </c>
-      <c r="I63" t="s">
-        <v>1</v>
-      </c>
-      <c r="J63">
-        <v>0.92</v>
-      </c>
-      <c r="K63" t="s">
-        <v>1</v>
-      </c>
-      <c r="L63">
+      <c r="D63" s="3">
+        <v>1.296</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F63" s="3">
+        <v>1.3773008</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H63" s="3">
+        <v>1.3953264000000001</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J63" s="3">
+        <v>0.99459509999999995</v>
+      </c>
+      <c r="K63" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L63" s="3">
         <v>0</v>
       </c>
       <c r="M63" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>29</v>
       </c>
       <c r="C64" t="s">
         <v>1</v>
       </c>
-      <c r="D64">
-        <v>-0.54700000000000004</v>
-      </c>
-      <c r="E64" t="s">
-        <v>1</v>
-      </c>
-      <c r="F64">
-        <v>1.375</v>
-      </c>
-      <c r="G64" t="s">
-        <v>1</v>
-      </c>
-      <c r="H64">
-        <v>1.3680000000000001</v>
-      </c>
-      <c r="I64" t="s">
-        <v>1</v>
-      </c>
-      <c r="J64">
-        <v>1.1020000000000001</v>
-      </c>
-      <c r="K64" t="s">
-        <v>1</v>
-      </c>
-      <c r="L64">
+      <c r="D64" s="3">
+        <v>-0.52800000000000002</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F64" s="3">
+        <v>1.0976811</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H64" s="3">
+        <v>1.1174343</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J64" s="3">
+        <v>1.1014649000000001</v>
+      </c>
+      <c r="K64" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L64" s="3">
         <v>0.88</v>
       </c>
       <c r="M64" s="2" t="s">
@@ -3095,32 +3378,32 @@
       <c r="C65" t="s">
         <v>1</v>
       </c>
-      <c r="D65">
-        <v>0.34300000000000003</v>
-      </c>
-      <c r="E65" t="s">
-        <v>1</v>
-      </c>
-      <c r="F65">
-        <v>2.089</v>
-      </c>
-      <c r="G65" t="s">
-        <v>1</v>
-      </c>
-      <c r="H65">
-        <v>2.335</v>
-      </c>
-      <c r="I65" t="s">
-        <v>1</v>
-      </c>
-      <c r="J65">
-        <v>1.048</v>
-      </c>
-      <c r="K65" t="s">
-        <v>1</v>
-      </c>
-      <c r="L65">
-        <v>0.16</v>
+      <c r="D65" s="3">
+        <v>-1.415</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F65" s="3">
+        <v>1.2896224000000001</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H65" s="3">
+        <v>1.3316786</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J65" s="3">
+        <v>1.0354251000000001</v>
+      </c>
+      <c r="K65" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L65" s="3">
+        <v>0.11</v>
       </c>
       <c r="M65" s="2" t="s">
         <v>22</v>
@@ -3130,11 +3413,29 @@
       <c r="B66" t="s">
         <v>20</v>
       </c>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
     </row>
     <row r="67" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>46</v>
       </c>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
       <c r="M67" s="2" t="s">
         <v>22</v>
       </c>
@@ -3143,6 +3444,15 @@
       <c r="B68" t="s">
         <v>20</v>
       </c>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
@@ -3151,32 +3461,32 @@
       <c r="C69" t="s">
         <v>1</v>
       </c>
-      <c r="D69">
-        <v>1.012</v>
-      </c>
-      <c r="E69" t="s">
-        <v>1</v>
-      </c>
-      <c r="F69">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="G69" t="s">
-        <v>1</v>
-      </c>
-      <c r="H69">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="I69" t="s">
-        <v>1</v>
-      </c>
-      <c r="J69">
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="K69" t="s">
-        <v>1</v>
-      </c>
-      <c r="L69">
-        <v>0.96</v>
+      <c r="D69" s="3">
+        <v>1.103</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F69" s="3">
+        <v>0.108</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H69" s="3">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J69" s="3">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="K69" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L69" s="3">
+        <v>0.11</v>
       </c>
       <c r="M69" s="2" t="s">
         <v>22</v>
@@ -3189,31 +3499,31 @@
       <c r="C70" t="s">
         <v>1</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="3">
         <v>-0.496</v>
       </c>
-      <c r="E70" t="s">
-        <v>1</v>
-      </c>
-      <c r="F70">
+      <c r="E70" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F70" s="3">
         <v>2.4E-2</v>
       </c>
-      <c r="G70" t="s">
-        <v>1</v>
-      </c>
-      <c r="H70">
-        <v>0.04</v>
-      </c>
-      <c r="I70" t="s">
-        <v>1</v>
-      </c>
-      <c r="J70">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="K70" t="s">
-        <v>1</v>
-      </c>
-      <c r="L70">
+      <c r="G70" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H70" s="3">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J70" s="3">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="K70" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L70" s="3">
         <v>0.94</v>
       </c>
       <c r="M70" s="2" t="s">
@@ -3227,32 +3537,32 @@
       <c r="C71" t="s">
         <v>1</v>
       </c>
-      <c r="D71">
-        <v>0.99199999999999999</v>
-      </c>
-      <c r="E71" t="s">
-        <v>1</v>
-      </c>
-      <c r="F71">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="G71" t="s">
-        <v>1</v>
-      </c>
-      <c r="H71">
-        <v>2.7E-2</v>
-      </c>
-      <c r="I71" t="s">
-        <v>1</v>
-      </c>
-      <c r="J71">
-        <v>0.113</v>
-      </c>
-      <c r="K71" t="s">
-        <v>1</v>
-      </c>
-      <c r="L71">
-        <v>0.9</v>
+      <c r="D71" s="3">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F71" s="3">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H71" s="3">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J71" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="K71" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L71" s="3">
+        <v>0.78</v>
       </c>
       <c r="M71" s="2" t="s">
         <v>22</v>
@@ -3262,11 +3572,29 @@
       <c r="B72" t="s">
         <v>20</v>
       </c>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
     </row>
     <row r="73" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>41</v>
       </c>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
       <c r="M73" s="2" t="s">
         <v>22</v>
       </c>
@@ -3275,28 +3603,51 @@
       <c r="B74" t="s">
         <v>20</v>
       </c>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
     </row>
     <row r="75" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C75" t="s">
         <v>1</v>
       </c>
-      <c r="E75" t="s">
-        <v>1</v>
-      </c>
-      <c r="F75" t="s">
+      <c r="D75" s="3"/>
+      <c r="E75" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F75" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K75" t="s">
-        <v>1</v>
-      </c>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L75" s="3"/>
       <c r="M75" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="76" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E76" t="s">
+      <c r="D76" s="3"/>
+      <c r="E76" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="3"/>
+      <c r="L76" s="3"/>
     </row>
     <row r="77" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
@@ -3305,31 +3656,31 @@
       <c r="C77" t="s">
         <v>1</v>
       </c>
-      <c r="D77">
-        <v>1.2350000000000001</v>
-      </c>
-      <c r="E77" t="s">
-        <v>1</v>
-      </c>
-      <c r="F77">
-        <v>6.9340000000000002</v>
-      </c>
-      <c r="G77" t="s">
-        <v>1</v>
-      </c>
-      <c r="H77">
-        <v>8.5280000000000005</v>
-      </c>
-      <c r="I77" t="s">
-        <v>1</v>
-      </c>
-      <c r="J77">
-        <v>0.77400000000000002</v>
-      </c>
-      <c r="K77" t="s">
-        <v>1</v>
-      </c>
-      <c r="L77">
+      <c r="D77" s="3">
+        <v>1.292</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" s="3">
+        <v>2.7065443</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H77" s="3">
+        <v>2.8297607</v>
+      </c>
+      <c r="I77" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J77" s="3">
+        <v>0.79159789999999997</v>
+      </c>
+      <c r="K77" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L77" s="3">
         <v>0</v>
       </c>
       <c r="M77" s="2" t="s">
@@ -3343,32 +3694,32 @@
       <c r="C78" t="s">
         <v>1</v>
       </c>
-      <c r="D78">
-        <v>-0.5</v>
-      </c>
-      <c r="E78" t="s">
-        <v>1</v>
-      </c>
-      <c r="F78">
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="G78" t="s">
-        <v>1</v>
-      </c>
-      <c r="H78">
-        <v>0.995</v>
-      </c>
-      <c r="I78" t="s">
-        <v>1</v>
-      </c>
-      <c r="J78">
-        <v>1.081</v>
-      </c>
-      <c r="K78" t="s">
-        <v>1</v>
-      </c>
-      <c r="L78">
-        <v>0.96</v>
+      <c r="D78" s="3">
+        <v>-0.501</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F78" s="3">
+        <v>1.0631028</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H78" s="3">
+        <v>1.0604313000000001</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J78" s="3">
+        <v>1.0870503</v>
+      </c>
+      <c r="K78" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L78" s="3">
+        <v>0.93</v>
       </c>
       <c r="M78" s="2" t="s">
         <v>22</v>
@@ -3381,32 +3732,32 @@
       <c r="C79" t="s">
         <v>1</v>
       </c>
-      <c r="D79">
-        <v>0.89400000000000002</v>
-      </c>
-      <c r="E79" t="s">
-        <v>1</v>
-      </c>
-      <c r="F79">
-        <v>3.3519999999999999</v>
-      </c>
-      <c r="G79" t="s">
-        <v>1</v>
-      </c>
-      <c r="H79">
-        <v>3.9660000000000002</v>
-      </c>
-      <c r="I79" t="s">
-        <v>1</v>
-      </c>
-      <c r="J79">
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="K79" t="s">
-        <v>1</v>
-      </c>
-      <c r="L79">
-        <v>0.01</v>
+      <c r="D79" s="3">
+        <v>1.266</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F79" s="3">
+        <v>4.1534582000000002</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H79" s="3">
+        <v>4.9138491999999996</v>
+      </c>
+      <c r="I79" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J79" s="3">
+        <v>0.8158533</v>
+      </c>
+      <c r="K79" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L79" s="3">
+        <v>0</v>
       </c>
       <c r="M79" s="2" t="s">
         <v>22</v>
@@ -3416,11 +3767,29 @@
       <c r="B80" t="s">
         <v>20</v>
       </c>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
     </row>
     <row r="81" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>42</v>
       </c>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
+      <c r="J81" s="3"/>
+      <c r="K81" s="3"/>
+      <c r="L81" s="3"/>
       <c r="M81" s="2" t="s">
         <v>22</v>
       </c>
@@ -3429,28 +3798,51 @@
       <c r="B82" t="s">
         <v>20</v>
       </c>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
     </row>
     <row r="83" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C83" t="s">
         <v>1</v>
       </c>
-      <c r="E83" t="s">
-        <v>1</v>
-      </c>
-      <c r="F83" t="s">
+      <c r="D83" s="3"/>
+      <c r="E83" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F83" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K83" t="s">
-        <v>1</v>
-      </c>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L83" s="3"/>
       <c r="M83" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="84" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E84" t="s">
+      <c r="D84" s="3"/>
+      <c r="E84" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="3"/>
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
+      <c r="L84" s="3"/>
     </row>
     <row r="85" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
@@ -3459,32 +3851,32 @@
       <c r="C85" t="s">
         <v>1</v>
       </c>
-      <c r="D85">
-        <v>1.026</v>
-      </c>
-      <c r="E85" t="s">
-        <v>1</v>
-      </c>
-      <c r="F85">
-        <v>1.5329999999999999</v>
-      </c>
-      <c r="G85" t="s">
-        <v>1</v>
-      </c>
-      <c r="H85">
-        <v>1.4750000000000001</v>
-      </c>
-      <c r="I85" t="s">
-        <v>1</v>
-      </c>
-      <c r="J85">
-        <v>1.2470000000000001</v>
-      </c>
-      <c r="K85" t="s">
-        <v>1</v>
-      </c>
-      <c r="L85">
-        <v>0.88</v>
+      <c r="D85" s="3">
+        <v>1.1559999999999999</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F85" s="3">
+        <v>1.4878199999999999</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H85" s="3">
+        <v>1.5142979999999999</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J85" s="3">
+        <v>1.2472532000000001</v>
+      </c>
+      <c r="K85" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L85" s="3">
+        <v>0.05</v>
       </c>
       <c r="M85" s="2" t="s">
         <v>22</v>
@@ -3497,32 +3889,32 @@
       <c r="C86" t="s">
         <v>1</v>
       </c>
-      <c r="D86">
-        <v>-0.49</v>
-      </c>
-      <c r="E86" t="s">
-        <v>1</v>
-      </c>
-      <c r="F86">
-        <v>1.409</v>
-      </c>
-      <c r="G86" t="s">
-        <v>1</v>
-      </c>
-      <c r="H86">
-        <v>1.3120000000000001</v>
-      </c>
-      <c r="I86" t="s">
-        <v>1</v>
-      </c>
-      <c r="J86">
-        <v>1.492</v>
-      </c>
-      <c r="K86" t="s">
-        <v>1</v>
-      </c>
-      <c r="L86">
-        <v>0.94</v>
+      <c r="D86" s="3">
+        <v>-0.41099999999999998</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F86" s="3">
+        <v>3.9880141999999998</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H86" s="3">
+        <v>4.7227759999999996</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J86" s="3">
+        <v>1.4669163999999999</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L86" s="3">
+        <v>0.27</v>
       </c>
       <c r="M86" s="2" t="s">
         <v>22</v>
@@ -3535,32 +3927,32 @@
       <c r="C87" t="s">
         <v>1</v>
       </c>
-      <c r="D87">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="E87" t="s">
-        <v>1</v>
-      </c>
-      <c r="F87">
-        <v>0.90200000000000002</v>
-      </c>
-      <c r="G87" t="s">
-        <v>1</v>
-      </c>
-      <c r="H87">
-        <v>0.90500000000000003</v>
-      </c>
-      <c r="I87" t="s">
-        <v>1</v>
-      </c>
-      <c r="J87">
-        <v>1.117</v>
-      </c>
-      <c r="K87" t="s">
-        <v>1</v>
-      </c>
-      <c r="L87">
-        <v>0.99</v>
+      <c r="D87" s="3">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F87" s="3">
+        <v>1.4213533</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H87" s="3">
+        <v>1.5066539999999999</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J87" s="3">
+        <v>1.0863649</v>
+      </c>
+      <c r="K87" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L87" s="3">
+        <v>0.56000000000000005</v>
       </c>
       <c r="M87" s="2" t="s">
         <v>22</v>
@@ -3570,11 +3962,29 @@
       <c r="B88" t="s">
         <v>20</v>
       </c>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
     </row>
     <row r="89" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>43</v>
       </c>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
+      <c r="K89" s="3"/>
+      <c r="L89" s="3"/>
       <c r="M89" s="2" t="s">
         <v>22</v>
       </c>
@@ -3583,28 +3993,51 @@
       <c r="B90" t="s">
         <v>20</v>
       </c>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="3"/>
     </row>
     <row r="91" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C91" t="s">
         <v>1</v>
       </c>
-      <c r="E91" t="s">
-        <v>1</v>
-      </c>
-      <c r="F91" t="s">
+      <c r="D91" s="3"/>
+      <c r="E91" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F91" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K91" t="s">
-        <v>1</v>
-      </c>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L91" s="3"/>
       <c r="M91" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="92" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E92" t="s">
+      <c r="D92" s="3"/>
+      <c r="E92" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
     </row>
     <row r="93" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
@@ -3613,31 +4046,31 @@
       <c r="C93" t="s">
         <v>1</v>
       </c>
-      <c r="D93">
-        <v>1.3540000000000001</v>
-      </c>
-      <c r="E93" t="s">
-        <v>1</v>
-      </c>
-      <c r="F93">
-        <v>10.406000000000001</v>
-      </c>
-      <c r="G93" t="s">
-        <v>1</v>
-      </c>
-      <c r="H93">
-        <v>12.843</v>
-      </c>
-      <c r="I93" t="s">
-        <v>1</v>
-      </c>
-      <c r="J93">
-        <v>0.67600000000000005</v>
-      </c>
-      <c r="K93" t="s">
-        <v>1</v>
-      </c>
-      <c r="L93">
+      <c r="D93" s="3">
+        <v>1.429</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F93" s="3">
+        <v>3.9738891999999999</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H93" s="3">
+        <v>4.1639643</v>
+      </c>
+      <c r="I93" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J93" s="3">
+        <v>0.68653679999999995</v>
+      </c>
+      <c r="K93" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L93" s="3">
         <v>0</v>
       </c>
       <c r="M93" s="2" t="s">
@@ -3651,32 +4084,32 @@
       <c r="C94" t="s">
         <v>1</v>
       </c>
-      <c r="D94">
-        <v>-0.496</v>
-      </c>
-      <c r="E94" t="s">
-        <v>1</v>
-      </c>
-      <c r="F94">
-        <v>1</v>
-      </c>
-      <c r="G94" t="s">
-        <v>1</v>
-      </c>
-      <c r="H94">
-        <v>0.997</v>
-      </c>
-      <c r="I94" t="s">
-        <v>1</v>
-      </c>
-      <c r="J94">
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="K94" t="s">
-        <v>1</v>
-      </c>
-      <c r="L94">
-        <v>0.92</v>
+      <c r="D94" s="3">
+        <v>-0.49199999999999999</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F94" s="3">
+        <v>1.0693573999999999</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H94" s="3">
+        <v>1.0863206000000001</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J94" s="3">
+        <v>1.0409904000000001</v>
+      </c>
+      <c r="K94" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L94" s="3">
+        <v>0.94</v>
       </c>
       <c r="M94" s="2" t="s">
         <v>22</v>
@@ -3689,32 +4122,32 @@
       <c r="C95" t="s">
         <v>1</v>
       </c>
-      <c r="D95">
-        <v>0.82299999999999995</v>
-      </c>
-      <c r="E95" t="s">
-        <v>1</v>
-      </c>
-      <c r="F95">
-        <v>5.5140000000000002</v>
-      </c>
-      <c r="G95" t="s">
-        <v>1</v>
-      </c>
-      <c r="H95">
-        <v>6.6159999999999997</v>
-      </c>
-      <c r="I95" t="s">
-        <v>1</v>
-      </c>
-      <c r="J95">
-        <v>0.89600000000000002</v>
-      </c>
-      <c r="K95" t="s">
-        <v>1</v>
-      </c>
-      <c r="L95">
-        <v>0</v>
+      <c r="D95" s="3">
+        <v>1.125</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F95" s="3">
+        <v>1.9828707000000001</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H95" s="3">
+        <v>2.3081873000000002</v>
+      </c>
+      <c r="I95" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J95" s="3">
+        <v>0.7330508</v>
+      </c>
+      <c r="K95" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L95" s="3">
+        <v>0.01</v>
       </c>
       <c r="M95" s="2" t="s">
         <v>22</v>
@@ -3767,5 +4200,6 @@
     <hyperlink ref="M67" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId39"/>
 </worksheet>
 </file>
</xml_diff>